<commit_message>
Primer Avance en Documento Personal de Investigación.
</commit_message>
<xml_diff>
--- a/Instrumento de Trabajo para Análisis de Lecturas.xlsx
+++ b/Instrumento de Trabajo para Análisis de Lecturas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\ESAP\Monitorias\tendencias de Administración Pública\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88964200-BFD1-45B4-BD4A-2FD133B48010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD7E9AE-2BC4-4A4B-8958-9A81648E4F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8475" yWindow="0" windowWidth="14610" windowHeight="15705" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FICHA DE LECTURA" sheetId="1" r:id="rId1"/>
@@ -750,6 +750,102 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -774,101 +870,8 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -893,9 +896,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1351,6 +1351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="E1:Y14"/>
   <sheetViews>
@@ -1634,8 +1635,9 @@
     <mergeCell ref="I8:R8"/>
     <mergeCell ref="I9:R9"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup scale="51" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1644,6 +1646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:W31"/>
   <sheetViews>
@@ -1736,28 +1739,28 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
       <c r="H7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="69"/>
-      <c r="R7" s="69"/>
-      <c r="S7" s="69"/>
-      <c r="T7" s="69"/>
-      <c r="U7" s="69"/>
-      <c r="V7" s="70"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
+      <c r="U7" s="49"/>
+      <c r="V7" s="50"/>
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1765,28 +1768,28 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="55" t="s">
+      <c r="E8" s="69"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="58" t="s">
+      <c r="I8" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="58"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
-      <c r="M8" s="59"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="60"/>
-      <c r="S8" s="60"/>
-      <c r="T8" s="60"/>
-      <c r="U8" s="60"/>
-      <c r="V8" s="61"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="45"/>
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1794,26 +1797,26 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="43" t="s">
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="43"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="45"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="45"/>
-      <c r="U9" s="45"/>
-      <c r="V9" s="46"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="39"/>
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1821,26 +1824,26 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="43" t="s">
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="43"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="45"/>
-      <c r="U10" s="45"/>
-      <c r="V10" s="46"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="38"/>
+      <c r="V10" s="39"/>
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1848,26 +1851,26 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="43" t="s">
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="43"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="45"/>
-      <c r="U11" s="45"/>
-      <c r="V11" s="46"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="38"/>
+      <c r="V11" s="39"/>
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1875,26 +1878,26 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="43" t="s">
+      <c r="E12" s="69"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="43"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="45"/>
-      <c r="R12" s="45"/>
-      <c r="S12" s="45"/>
-      <c r="T12" s="45"/>
-      <c r="U12" s="45"/>
-      <c r="V12" s="46"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="38"/>
+      <c r="T12" s="38"/>
+      <c r="U12" s="38"/>
+      <c r="V12" s="39"/>
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1902,26 +1905,26 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="43" t="s">
+      <c r="E13" s="69"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="43"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="46"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="38"/>
+      <c r="T13" s="38"/>
+      <c r="U13" s="38"/>
+      <c r="V13" s="39"/>
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1929,26 +1932,26 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="43" t="s">
+      <c r="E14" s="69"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="43"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="45"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="46"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="38"/>
+      <c r="T14" s="38"/>
+      <c r="U14" s="38"/>
+      <c r="V14" s="39"/>
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:23" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1956,26 +1959,26 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="47" t="s">
+      <c r="E15" s="69"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="47"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49"/>
-      <c r="Q15" s="49"/>
-      <c r="R15" s="49"/>
-      <c r="S15" s="49"/>
-      <c r="T15" s="49"/>
-      <c r="U15" s="49"/>
-      <c r="V15" s="50"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="41"/>
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1983,28 +1986,28 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="66" t="s">
+      <c r="E16" s="69"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="71" t="s">
+      <c r="I16" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="71"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="73"/>
-      <c r="O16" s="73"/>
-      <c r="P16" s="73"/>
-      <c r="Q16" s="73"/>
-      <c r="R16" s="73"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="73"/>
-      <c r="U16" s="73"/>
-      <c r="V16" s="74"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="53"/>
+      <c r="S16" s="53"/>
+      <c r="T16" s="53"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="54"/>
       <c r="W16" s="2"/>
     </row>
     <row r="17" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2012,26 +2015,26 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="51" t="s">
+      <c r="E17" s="69"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="51"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="53"/>
-      <c r="P17" s="53"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="53"/>
-      <c r="T17" s="53"/>
-      <c r="U17" s="53"/>
-      <c r="V17" s="54"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="58"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="58"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="58"/>
+      <c r="U17" s="58"/>
+      <c r="V17" s="59"/>
       <c r="W17" s="2"/>
     </row>
     <row r="18" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2039,26 +2042,26 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="51" t="s">
+      <c r="E18" s="69"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="J18" s="51"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="53"/>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="53"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="53"/>
-      <c r="V18" s="54"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="58"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="58"/>
+      <c r="Q18" s="58"/>
+      <c r="R18" s="58"/>
+      <c r="S18" s="58"/>
+      <c r="T18" s="58"/>
+      <c r="U18" s="58"/>
+      <c r="V18" s="59"/>
       <c r="W18" s="2"/>
     </row>
     <row r="19" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2066,26 +2069,26 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="51" t="s">
+      <c r="E19" s="69"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="J19" s="51"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="53"/>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-      <c r="V19" s="54"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="58"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="58"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="58"/>
+      <c r="U19" s="58"/>
+      <c r="V19" s="59"/>
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2093,26 +2096,26 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="51" t="s">
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="51"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="53"/>
-      <c r="O20" s="53"/>
-      <c r="P20" s="53"/>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="53"/>
-      <c r="S20" s="53"/>
-      <c r="T20" s="53"/>
-      <c r="U20" s="53"/>
-      <c r="V20" s="54"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="57"/>
+      <c r="M20" s="57"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="58"/>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="58"/>
+      <c r="T20" s="58"/>
+      <c r="U20" s="58"/>
+      <c r="V20" s="59"/>
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2120,26 +2123,26 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="51" t="s">
+      <c r="E21" s="69"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="51"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="53"/>
-      <c r="P21" s="53"/>
-      <c r="Q21" s="53"/>
-      <c r="R21" s="53"/>
-      <c r="S21" s="53"/>
-      <c r="T21" s="53"/>
-      <c r="U21" s="53"/>
-      <c r="V21" s="54"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="57"/>
+      <c r="M21" s="57"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="58"/>
+      <c r="Q21" s="58"/>
+      <c r="R21" s="58"/>
+      <c r="S21" s="58"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="V21" s="59"/>
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2147,26 +2150,26 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="51" t="s">
+      <c r="E22" s="69"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="51"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="53"/>
-      <c r="P22" s="53"/>
-      <c r="Q22" s="53"/>
-      <c r="R22" s="53"/>
-      <c r="S22" s="53"/>
-      <c r="T22" s="53"/>
-      <c r="U22" s="53"/>
-      <c r="V22" s="54"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="58"/>
+      <c r="Q22" s="58"/>
+      <c r="R22" s="58"/>
+      <c r="S22" s="58"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="59"/>
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2174,26 +2177,26 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="62" t="s">
+      <c r="E23" s="69"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="62"/>
-      <c r="K23" s="63"/>
-      <c r="L23" s="63"/>
-      <c r="M23" s="63"/>
-      <c r="N23" s="64"/>
-      <c r="O23" s="64"/>
-      <c r="P23" s="64"/>
-      <c r="Q23" s="64"/>
-      <c r="R23" s="64"/>
-      <c r="S23" s="64"/>
-      <c r="T23" s="64"/>
-      <c r="U23" s="64"/>
-      <c r="V23" s="65"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="65"/>
+      <c r="O23" s="65"/>
+      <c r="P23" s="65"/>
+      <c r="Q23" s="65"/>
+      <c r="R23" s="65"/>
+      <c r="S23" s="65"/>
+      <c r="T23" s="65"/>
+      <c r="U23" s="65"/>
+      <c r="V23" s="66"/>
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2201,28 +2204,28 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="55" t="s">
+      <c r="E24" s="69"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="58" t="s">
+      <c r="I24" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="58"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="60"/>
-      <c r="O24" s="60"/>
-      <c r="P24" s="60"/>
-      <c r="Q24" s="60"/>
-      <c r="R24" s="60"/>
-      <c r="S24" s="60"/>
-      <c r="T24" s="60"/>
-      <c r="U24" s="60"/>
-      <c r="V24" s="61"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="44"/>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="44"/>
+      <c r="T24" s="44"/>
+      <c r="U24" s="44"/>
+      <c r="V24" s="45"/>
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2230,26 +2233,26 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="43" t="s">
+      <c r="E25" s="69"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="43"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="45"/>
-      <c r="R25" s="45"/>
-      <c r="S25" s="45"/>
-      <c r="T25" s="45"/>
-      <c r="U25" s="45"/>
-      <c r="V25" s="46"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="38"/>
+      <c r="U25" s="38"/>
+      <c r="V25" s="39"/>
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2257,26 +2260,26 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="43" t="s">
+      <c r="E26" s="69"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="J26" s="43"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45"/>
-      <c r="V26" s="46"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
+      <c r="S26" s="38"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="38"/>
+      <c r="V26" s="39"/>
       <c r="W26" s="2"/>
     </row>
     <row r="27" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2284,26 +2287,26 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="43" t="s">
+      <c r="E27" s="69"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="43"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="45"/>
-      <c r="Q27" s="45"/>
-      <c r="R27" s="45"/>
-      <c r="S27" s="45"/>
-      <c r="T27" s="45"/>
-      <c r="U27" s="45"/>
-      <c r="V27" s="46"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="38"/>
+      <c r="T27" s="38"/>
+      <c r="U27" s="38"/>
+      <c r="V27" s="39"/>
       <c r="W27" s="2"/>
     </row>
     <row r="28" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2311,26 +2314,26 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="43" t="s">
+      <c r="E28" s="69"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="43"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="45"/>
-      <c r="U28" s="45"/>
-      <c r="V28" s="46"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="38"/>
+      <c r="R28" s="38"/>
+      <c r="S28" s="38"/>
+      <c r="T28" s="38"/>
+      <c r="U28" s="38"/>
+      <c r="V28" s="39"/>
       <c r="W28" s="2"/>
     </row>
     <row r="29" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2338,26 +2341,26 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="43" t="s">
+      <c r="E29" s="69"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="43"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="45"/>
-      <c r="U29" s="45"/>
-      <c r="V29" s="46"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="38"/>
+      <c r="S29" s="38"/>
+      <c r="T29" s="38"/>
+      <c r="U29" s="38"/>
+      <c r="V29" s="39"/>
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2365,26 +2368,26 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="43" t="s">
+      <c r="E30" s="69"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="J30" s="43"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="45"/>
-      <c r="T30" s="45"/>
-      <c r="U30" s="45"/>
-      <c r="V30" s="46"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="38"/>
+      <c r="T30" s="38"/>
+      <c r="U30" s="38"/>
+      <c r="V30" s="39"/>
       <c r="W30" s="2"/>
     </row>
     <row r="31" spans="1:23" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2392,30 +2395,94 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="47" t="s">
+      <c r="E31" s="72"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="J31" s="47"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="48"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="49"/>
-      <c r="T31" s="49"/>
-      <c r="U31" s="49"/>
-      <c r="V31" s="50"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="40"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="40"/>
+      <c r="Q31" s="40"/>
+      <c r="R31" s="40"/>
+      <c r="S31" s="40"/>
+      <c r="T31" s="40"/>
+      <c r="U31" s="40"/>
+      <c r="V31" s="41"/>
       <c r="W31" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="E7:G31"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="N29:V29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="N30:V30"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="N28:V28"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="N31:V31"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="N25:V25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="N26:V26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="N27:V27"/>
+    <mergeCell ref="N22:V22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:V23"/>
+    <mergeCell ref="H24:H31"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:V24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="N17:V17"/>
+    <mergeCell ref="H16:H23"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="N18:V18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="N19:V19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="N20:V20"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="N21:V21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="H8:H15"/>
+    <mergeCell ref="I7:V7"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="N16:V16"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:M11"/>
     <mergeCell ref="H6:Q6"/>
     <mergeCell ref="K8:M8"/>
     <mergeCell ref="I14:J14"/>
@@ -2432,78 +2499,19 @@
     <mergeCell ref="N9:V9"/>
     <mergeCell ref="N10:V10"/>
     <mergeCell ref="N11:V11"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="H8:H15"/>
-    <mergeCell ref="I7:V7"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="N16:V16"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="N17:V17"/>
-    <mergeCell ref="H16:H23"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="N18:V18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="N19:V19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="N20:V20"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="N21:V21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="H24:H31"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:V24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="N26:V26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="N27:V27"/>
-    <mergeCell ref="N22:V22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:V23"/>
-    <mergeCell ref="E7:G31"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="N29:V29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="N30:V30"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="N28:V28"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="N31:V31"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="N25:V25"/>
-    <mergeCell ref="I26:J26"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="45" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:W30"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -2596,28 +2604,28 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="83"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="75"/>
       <c r="H7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="75"/>
-      <c r="M7" s="75"/>
-      <c r="N7" s="75"/>
-      <c r="O7" s="75"/>
-      <c r="P7" s="75"/>
-      <c r="Q7" s="75"/>
-      <c r="R7" s="75"/>
-      <c r="S7" s="75"/>
-      <c r="T7" s="75"/>
-      <c r="U7" s="75"/>
-      <c r="V7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="76"/>
+      <c r="O7" s="76"/>
+      <c r="P7" s="76"/>
+      <c r="Q7" s="76"/>
+      <c r="R7" s="76"/>
+      <c r="S7" s="76"/>
+      <c r="T7" s="76"/>
+      <c r="U7" s="76"/>
+      <c r="V7" s="77"/>
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2625,26 +2633,26 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="39"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="71"/>
       <c r="H8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="75"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="75"/>
-      <c r="Q8" s="75"/>
-      <c r="R8" s="75"/>
-      <c r="S8" s="75"/>
-      <c r="T8" s="75"/>
-      <c r="U8" s="75"/>
-      <c r="V8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="76"/>
+      <c r="O8" s="76"/>
+      <c r="P8" s="76"/>
+      <c r="Q8" s="76"/>
+      <c r="R8" s="76"/>
+      <c r="S8" s="76"/>
+      <c r="T8" s="76"/>
+      <c r="U8" s="76"/>
+      <c r="V8" s="77"/>
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2652,26 +2660,26 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="39"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="71"/>
       <c r="H9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="75"/>
-      <c r="S9" s="75"/>
-      <c r="T9" s="75"/>
-      <c r="U9" s="75"/>
-      <c r="V9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="76"/>
+      <c r="S9" s="76"/>
+      <c r="T9" s="76"/>
+      <c r="U9" s="76"/>
+      <c r="V9" s="77"/>
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2679,28 +2687,28 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="55" t="s">
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="58" t="s">
+      <c r="I10" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="58"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
-      <c r="T10" s="60"/>
-      <c r="U10" s="60"/>
-      <c r="V10" s="61"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="44"/>
+      <c r="T10" s="44"/>
+      <c r="U10" s="44"/>
+      <c r="V10" s="45"/>
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2708,26 +2716,26 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="43" t="s">
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="43"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="45"/>
-      <c r="U11" s="45"/>
-      <c r="V11" s="46"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="38"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="38"/>
+      <c r="V11" s="39"/>
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2735,26 +2743,26 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="43" t="s">
+      <c r="E12" s="69"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="43"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="44"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="45"/>
-      <c r="R12" s="45"/>
-      <c r="S12" s="45"/>
-      <c r="T12" s="45"/>
-      <c r="U12" s="45"/>
-      <c r="V12" s="46"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="38"/>
+      <c r="T12" s="38"/>
+      <c r="U12" s="38"/>
+      <c r="V12" s="39"/>
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2762,26 +2770,26 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="43" t="s">
+      <c r="E13" s="69"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="43"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="46"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="38"/>
+      <c r="T13" s="38"/>
+      <c r="U13" s="38"/>
+      <c r="V13" s="39"/>
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2789,26 +2797,26 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="47" t="s">
+      <c r="E14" s="69"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="J14" s="47"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="49"/>
-      <c r="S14" s="49"/>
-      <c r="T14" s="49"/>
-      <c r="U14" s="49"/>
-      <c r="V14" s="50"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="41"/>
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2816,26 +2824,26 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="66" t="s">
+      <c r="E15" s="69"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="77"/>
-      <c r="N15" s="77"/>
-      <c r="O15" s="77"/>
-      <c r="P15" s="77"/>
-      <c r="Q15" s="77"/>
-      <c r="R15" s="77"/>
-      <c r="S15" s="77"/>
-      <c r="T15" s="77"/>
-      <c r="U15" s="77"/>
-      <c r="V15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="78"/>
+      <c r="N15" s="78"/>
+      <c r="O15" s="78"/>
+      <c r="P15" s="78"/>
+      <c r="Q15" s="78"/>
+      <c r="R15" s="78"/>
+      <c r="S15" s="78"/>
+      <c r="T15" s="78"/>
+      <c r="U15" s="78"/>
+      <c r="V15" s="79"/>
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2843,24 +2851,24 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="79"/>
-      <c r="K16" s="79"/>
-      <c r="L16" s="79"/>
-      <c r="M16" s="79"/>
-      <c r="N16" s="79"/>
-      <c r="O16" s="79"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="79"/>
-      <c r="R16" s="79"/>
-      <c r="S16" s="79"/>
-      <c r="T16" s="79"/>
-      <c r="U16" s="79"/>
-      <c r="V16" s="80"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
+      <c r="L16" s="80"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="80"/>
+      <c r="O16" s="80"/>
+      <c r="P16" s="80"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="80"/>
+      <c r="S16" s="80"/>
+      <c r="T16" s="80"/>
+      <c r="U16" s="80"/>
+      <c r="V16" s="81"/>
       <c r="W16" s="2"/>
     </row>
     <row r="17" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2868,24 +2876,24 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="79"/>
-      <c r="P17" s="79"/>
-      <c r="Q17" s="79"/>
-      <c r="R17" s="79"/>
-      <c r="S17" s="79"/>
-      <c r="T17" s="79"/>
-      <c r="U17" s="79"/>
-      <c r="V17" s="80"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="80"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="80"/>
+      <c r="O17" s="80"/>
+      <c r="P17" s="80"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="80"/>
+      <c r="S17" s="80"/>
+      <c r="T17" s="80"/>
+      <c r="U17" s="80"/>
+      <c r="V17" s="81"/>
       <c r="W17" s="2"/>
     </row>
     <row r="18" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2893,24 +2901,24 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="79"/>
-      <c r="K18" s="79"/>
-      <c r="L18" s="79"/>
-      <c r="M18" s="79"/>
-      <c r="N18" s="79"/>
-      <c r="O18" s="79"/>
-      <c r="P18" s="79"/>
-      <c r="Q18" s="79"/>
-      <c r="R18" s="79"/>
-      <c r="S18" s="79"/>
-      <c r="T18" s="79"/>
-      <c r="U18" s="79"/>
-      <c r="V18" s="80"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="80"/>
+      <c r="L18" s="80"/>
+      <c r="M18" s="80"/>
+      <c r="N18" s="80"/>
+      <c r="O18" s="80"/>
+      <c r="P18" s="80"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="80"/>
+      <c r="S18" s="80"/>
+      <c r="T18" s="80"/>
+      <c r="U18" s="80"/>
+      <c r="V18" s="81"/>
       <c r="W18" s="2"/>
     </row>
     <row r="19" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2918,24 +2926,24 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="79"/>
-      <c r="L19" s="79"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="79"/>
-      <c r="P19" s="79"/>
-      <c r="Q19" s="79"/>
-      <c r="R19" s="79"/>
-      <c r="S19" s="79"/>
-      <c r="T19" s="79"/>
-      <c r="U19" s="79"/>
-      <c r="V19" s="80"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="80"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="80"/>
+      <c r="O19" s="80"/>
+      <c r="P19" s="80"/>
+      <c r="Q19" s="80"/>
+      <c r="R19" s="80"/>
+      <c r="S19" s="80"/>
+      <c r="T19" s="80"/>
+      <c r="U19" s="80"/>
+      <c r="V19" s="81"/>
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2943,24 +2951,24 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="79"/>
-      <c r="J20" s="79"/>
-      <c r="K20" s="79"/>
-      <c r="L20" s="79"/>
-      <c r="M20" s="79"/>
-      <c r="N20" s="79"/>
-      <c r="O20" s="79"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="79"/>
-      <c r="S20" s="79"/>
-      <c r="T20" s="79"/>
-      <c r="U20" s="79"/>
-      <c r="V20" s="80"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="80"/>
+      <c r="M20" s="80"/>
+      <c r="N20" s="80"/>
+      <c r="O20" s="80"/>
+      <c r="P20" s="80"/>
+      <c r="Q20" s="80"/>
+      <c r="R20" s="80"/>
+      <c r="S20" s="80"/>
+      <c r="T20" s="80"/>
+      <c r="U20" s="80"/>
+      <c r="V20" s="81"/>
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2968,24 +2976,24 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="79"/>
-      <c r="J21" s="79"/>
-      <c r="K21" s="79"/>
-      <c r="L21" s="79"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="79"/>
-      <c r="P21" s="79"/>
-      <c r="Q21" s="79"/>
-      <c r="R21" s="79"/>
-      <c r="S21" s="79"/>
-      <c r="T21" s="79"/>
-      <c r="U21" s="79"/>
-      <c r="V21" s="80"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="80"/>
+      <c r="K21" s="80"/>
+      <c r="L21" s="80"/>
+      <c r="M21" s="80"/>
+      <c r="N21" s="80"/>
+      <c r="O21" s="80"/>
+      <c r="P21" s="80"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="80"/>
+      <c r="S21" s="80"/>
+      <c r="T21" s="80"/>
+      <c r="U21" s="80"/>
+      <c r="V21" s="81"/>
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2993,24 +3001,24 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="81"/>
-      <c r="O22" s="81"/>
-      <c r="P22" s="81"/>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="81"/>
-      <c r="S22" s="81"/>
-      <c r="T22" s="81"/>
-      <c r="U22" s="81"/>
-      <c r="V22" s="82"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="82"/>
+      <c r="R22" s="82"/>
+      <c r="S22" s="82"/>
+      <c r="T22" s="82"/>
+      <c r="U22" s="82"/>
+      <c r="V22" s="83"/>
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3018,28 +3026,28 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="55" t="s">
+      <c r="E23" s="69"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="I23" s="58" t="s">
+      <c r="I23" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="J23" s="58"/>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="60"/>
-      <c r="T23" s="60"/>
-      <c r="U23" s="60"/>
-      <c r="V23" s="61"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="44"/>
+      <c r="Q23" s="44"/>
+      <c r="R23" s="44"/>
+      <c r="S23" s="44"/>
+      <c r="T23" s="44"/>
+      <c r="U23" s="44"/>
+      <c r="V23" s="45"/>
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3047,26 +3055,26 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="43" t="s">
+      <c r="E24" s="69"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="J24" s="43"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="45"/>
-      <c r="Q24" s="45"/>
-      <c r="R24" s="45"/>
-      <c r="S24" s="45"/>
-      <c r="T24" s="45"/>
-      <c r="U24" s="45"/>
-      <c r="V24" s="46"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+      <c r="S24" s="38"/>
+      <c r="T24" s="38"/>
+      <c r="U24" s="38"/>
+      <c r="V24" s="39"/>
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3074,26 +3082,26 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="43" t="s">
+      <c r="E25" s="69"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="J25" s="43"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="45"/>
-      <c r="R25" s="45"/>
-      <c r="S25" s="45"/>
-      <c r="T25" s="45"/>
-      <c r="U25" s="45"/>
-      <c r="V25" s="46"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="38"/>
+      <c r="U25" s="38"/>
+      <c r="V25" s="39"/>
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3101,26 +3109,26 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="43" t="s">
+      <c r="E26" s="69"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="J26" s="43"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45"/>
-      <c r="V26" s="46"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
+      <c r="S26" s="38"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="38"/>
+      <c r="V26" s="39"/>
       <c r="W26" s="2"/>
     </row>
     <row r="27" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3128,26 +3136,26 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="43" t="s">
+      <c r="E27" s="69"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="J27" s="43"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="45"/>
-      <c r="Q27" s="45"/>
-      <c r="R27" s="45"/>
-      <c r="S27" s="45"/>
-      <c r="T27" s="45"/>
-      <c r="U27" s="45"/>
-      <c r="V27" s="46"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="38"/>
+      <c r="T27" s="38"/>
+      <c r="U27" s="38"/>
+      <c r="V27" s="39"/>
       <c r="W27" s="2"/>
     </row>
     <row r="28" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3155,26 +3163,26 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="43" t="s">
+      <c r="E28" s="69"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="J28" s="43"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="45"/>
-      <c r="U28" s="45"/>
-      <c r="V28" s="46"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="38"/>
+      <c r="R28" s="38"/>
+      <c r="S28" s="38"/>
+      <c r="T28" s="38"/>
+      <c r="U28" s="38"/>
+      <c r="V28" s="39"/>
       <c r="W28" s="2"/>
     </row>
     <row r="29" spans="1:23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3182,26 +3190,26 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="43" t="s">
+      <c r="E29" s="69"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="43"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="45"/>
-      <c r="U29" s="45"/>
-      <c r="V29" s="46"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="38"/>
+      <c r="S29" s="38"/>
+      <c r="T29" s="38"/>
+      <c r="U29" s="38"/>
+      <c r="V29" s="39"/>
       <c r="W29" s="2"/>
     </row>
     <row r="30" spans="1:23" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3209,30 +3217,64 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="47" t="s">
+      <c r="E30" s="72"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="J30" s="47"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="49"/>
-      <c r="T30" s="49"/>
-      <c r="U30" s="49"/>
-      <c r="V30" s="50"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
+      <c r="R30" s="40"/>
+      <c r="S30" s="40"/>
+      <c r="T30" s="40"/>
+      <c r="U30" s="40"/>
+      <c r="V30" s="41"/>
       <c r="W30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="N26:V26"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="N29:V29"/>
+    <mergeCell ref="N25:V25"/>
+    <mergeCell ref="N24:V24"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="N27:V27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="N28:V28"/>
+    <mergeCell ref="H1:R1"/>
+    <mergeCell ref="H2:R2"/>
+    <mergeCell ref="H6:Q6"/>
+    <mergeCell ref="I7:V7"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:V23"/>
+    <mergeCell ref="I8:V8"/>
+    <mergeCell ref="I9:V9"/>
+    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="I15:V22"/>
+    <mergeCell ref="H23:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="N30:V30"/>
+    <mergeCell ref="I27:J27"/>
     <mergeCell ref="E7:G30"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="K10:M10"/>
@@ -3249,42 +3291,10 @@
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="N13:V13"/>
-    <mergeCell ref="H1:R1"/>
-    <mergeCell ref="H2:R2"/>
-    <mergeCell ref="H6:Q6"/>
-    <mergeCell ref="I7:V7"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:V23"/>
-    <mergeCell ref="I8:V8"/>
-    <mergeCell ref="I9:V9"/>
-    <mergeCell ref="H10:H14"/>
-    <mergeCell ref="I15:V22"/>
-    <mergeCell ref="H23:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="N30:V30"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="N27:V27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="N28:V28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="N29:V29"/>
-    <mergeCell ref="N25:V25"/>
-    <mergeCell ref="N24:V24"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="N26:V26"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="K25:M25"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="44" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>